<commit_message>
revision 1.2 ajouté détection de fautes, dipswitch, connecteur WIFI, etc.
</commit_message>
<xml_diff>
--- a/calculs.xlsx
+++ b/calculs.xlsx
@@ -5,19 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laf\OneDrive\05_Technolaf\borne_l2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laf\OneDrive\05_Technolaf\evse_technolaf_hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{867CA2C8-9198-48F2-91CF-A000E97D3030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17593D8-B4B0-4227-9EF6-83E9AB63FFBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-6990" windowWidth="21840" windowHeight="13740" xr2:uid="{046B47D2-9F1C-41FF-8AA1-9D5891615543}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{046B47D2-9F1C-41FF-8AA1-9D5891615543}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="IIR" sheetId="2" r:id="rId2"/>
+    <sheet name="Vmeas" sheetId="3" r:id="rId3"/>
+    <sheet name="dip_sw" sheetId="5" r:id="rId4"/>
+    <sheet name="Imeas" sheetId="4" r:id="rId5"/>
+    <sheet name="gfi" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
   <si>
     <t>Mhz</t>
   </si>
@@ -124,11 +127,128 @@
   <si>
     <t>OVERFLOW time elapsed</t>
   </si>
+  <si>
+    <t>peak</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>Vmeas</t>
+  </si>
+  <si>
+    <t>vd</t>
+  </si>
+  <si>
+    <t>Vadc</t>
+  </si>
+  <si>
+    <t>nF</t>
+  </si>
+  <si>
+    <t>test R</t>
+  </si>
+  <si>
+    <t>peak V</t>
+  </si>
+  <si>
+    <t>source peak</t>
+  </si>
+  <si>
+    <t>new R</t>
+  </si>
+  <si>
+    <t>new V</t>
+  </si>
+  <si>
+    <t>Rdiode</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>mV</t>
+  </si>
+  <si>
+    <t>uA</t>
+  </si>
+  <si>
+    <t>vline_rms</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>duty %</t>
+  </si>
+  <si>
+    <t>I clamp on meter</t>
+  </si>
+  <si>
+    <t>ibody</t>
+  </si>
+  <si>
+    <t>V L-N</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Pr</t>
+  </si>
+  <si>
+    <t>Iset</t>
+  </si>
+  <si>
+    <t>I calc</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>V (4 mA)</t>
+  </si>
+  <si>
+    <t>V (2 uA)</t>
+  </si>
+  <si>
+    <t>PA4(100R)</t>
+  </si>
+  <si>
+    <t>PA4(270R)</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>Amps</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,11 +293,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,7 +756,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$E$4:$E$304</c:f>
+              <c:f>IIR!$E$4:$E$304</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="301"/>
@@ -1542,7 +1668,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$G$4:$G$304</c:f>
+              <c:f>IIR!$G$4:$G$304</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="301"/>
@@ -2620,6 +2746,455 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.161980030370865"/>
+                  <c:y val="-6.7992768915412949E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Imeas!$E$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Imeas!$E$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1588</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1935</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AE55-4B5E-9F62-EA9C7B4B0F8B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent2"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Imeas!$E$2:$J$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Imeas!$E$9:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.23600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43828571428571433</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60685714285714287</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80914285714285727</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0114285714285716</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6182857142857145</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AE55-4B5E-9F62-EA9C7B4B0F8B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="378843176"/>
+        <c:axId val="378840224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="378843176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378840224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="378840224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378843176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2661,6 +3236,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3732,6 +4347,541 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="100" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="79000">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="60000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3794,6 +4944,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97137CB2-B785-4683-BF94-B4CBF8E212D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7496FB7-35EE-4EA7-9C20-382B5B5DA551}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4113,8 +5304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66288A62-13E5-4C8D-B2A6-AB885FF610D1}">
   <dimension ref="B1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4804,8 +5995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3063F6-7DB3-4706-9607-D4AB253AA7FA}">
   <dimension ref="D1:O503"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28:I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12878,4 +14069,1439 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E33E340B-BDD3-48B5-B133-018F36174080}">
+  <dimension ref="A2:N18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>240</v>
+      </c>
+      <c r="C2">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>120</v>
+      </c>
+      <c r="C4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <f>B4*SQRT(2)</f>
+        <v>169.70562748477141</v>
+      </c>
+      <c r="C5">
+        <f>C4*SQRT(2)</f>
+        <v>169.70562748477141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6">
+        <f>240*1.25</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E7" s="4">
+        <f>B7*E6</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B6/(B6+B7)</f>
+        <v>9.9009900990099011E-3</v>
+      </c>
+      <c r="C8" s="1">
+        <f>C6/(C6+C7)</f>
+        <v>9.9009900990099011E-3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="4">
+        <f>B5*B8</f>
+        <v>1.6802537374729842</v>
+      </c>
+      <c r="C9" s="4">
+        <f>C5*C8</f>
+        <v>1.6802537374729842</v>
+      </c>
+      <c r="J9">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="K9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="4">
+        <f>B9-B10</f>
+        <v>1.1802537374729842</v>
+      </c>
+      <c r="C11" s="4">
+        <f>C9-C10</f>
+        <v>1.1802537374729842</v>
+      </c>
+      <c r="J11" s="1">
+        <f>J9/J8</f>
+        <v>5.6499999999999999E-7</v>
+      </c>
+      <c r="K11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <f>B11*1000</f>
+        <v>1180.2537374729843</v>
+      </c>
+      <c r="C12">
+        <f>C11*1000</f>
+        <v>1180.2537374729843</v>
+      </c>
+      <c r="D12">
+        <v>550</v>
+      </c>
+      <c r="J12" s="4">
+        <f>J11*1000000</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="K12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f>B12*2-1000</f>
+        <v>1360.5074749459686</v>
+      </c>
+      <c r="C14">
+        <f>C12-500</f>
+        <v>680.25373747298431</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15">
+        <f>B14/5.67</f>
+        <v>239.94840827971228</v>
+      </c>
+      <c r="C15">
+        <f>C14/5.67</f>
+        <v>119.97420413985614</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>B14/(2*B4)</f>
+        <v>5.6687811456082029</v>
+      </c>
+      <c r="I16">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>565</v>
+      </c>
+      <c r="I17">
+        <f>I16/1000000</f>
+        <v>1.7000000000000001E-4</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>B17/10</f>
+        <v>56.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4E0E3F-7AF1-417F-87DD-04F1A027EFD5}">
+  <dimension ref="B1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="6" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <f>IF(_xlfn.BITAND($B2,8)&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <f>IF(_xlfn.BITAND($B2,4)&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <f>IF(_xlfn.BITAND($B2,2)&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <f>IF(_xlfn.BITAND($B2,1)&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="7">
+        <f>(B2+1)*3.2</f>
+        <v>3.2</v>
+      </c>
+      <c r="H2" s="6">
+        <f>G2/0.6</f>
+        <v>5.3333333333333339</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C17" si="0">IF(_xlfn.BITAND($B3,8)&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D17" si="1">IF(_xlfn.BITAND($B3,4)&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E17" si="2">IF(_xlfn.BITAND($B3,2)&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F17" si="3">IF(_xlfn.BITAND($B3,1)&lt;&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:G16" si="4">(B3+1)*3.2</f>
+        <v>6.4</v>
+      </c>
+      <c r="H3" s="6">
+        <f t="shared" ref="H3:H17" si="5">G3/0.6</f>
+        <v>10.666666666666668</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="4"/>
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" si="5"/>
+        <v>16.000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="4"/>
+        <v>12.8</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" si="5"/>
+        <v>21.333333333333336</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="5"/>
+        <v>26.666666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="4"/>
+        <v>19.200000000000003</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="5"/>
+        <v>32.000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="4"/>
+        <v>22.400000000000002</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="5"/>
+        <v>37.333333333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="4"/>
+        <v>25.6</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="5"/>
+        <v>42.666666666666671</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="4"/>
+        <v>28.8</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="5"/>
+        <v>53.333333333333336</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="4"/>
+        <v>35.200000000000003</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="5"/>
+        <v>58.666666666666671</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="4"/>
+        <v>38.400000000000006</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="5"/>
+        <v>64.000000000000014</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="4"/>
+        <v>41.6</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="5"/>
+        <v>69.333333333333343</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="4"/>
+        <v>44.800000000000004</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="5"/>
+        <v>74.666666666666671</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="7">
+        <v>26</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="5"/>
+        <v>43.333333333333336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B07A46-EA4B-4BD4-89DB-935E46C70620}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1">
+        <v>7</v>
+      </c>
+      <c r="F1">
+        <v>13</v>
+      </c>
+      <c r="G1">
+        <v>18</v>
+      </c>
+      <c r="H1">
+        <v>24</v>
+      </c>
+      <c r="I1">
+        <v>30</v>
+      </c>
+      <c r="J1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>25.3</v>
+      </c>
+      <c r="E2">
+        <v>6.5</v>
+      </c>
+      <c r="F2">
+        <v>11.8</v>
+      </c>
+      <c r="G2">
+        <v>17.3</v>
+      </c>
+      <c r="H2">
+        <v>23.4</v>
+      </c>
+      <c r="I2">
+        <v>28.8</v>
+      </c>
+      <c r="J2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>50.4</v>
+      </c>
+      <c r="E4">
+        <v>23.6</v>
+      </c>
+      <c r="F4">
+        <f>$E4*F1/$E1</f>
+        <v>43.828571428571429</v>
+      </c>
+      <c r="G4">
+        <f>$E4*G1/$E1</f>
+        <v>60.68571428571429</v>
+      </c>
+      <c r="H4">
+        <f>$E4*H1/$E1</f>
+        <v>80.914285714285725</v>
+      </c>
+      <c r="I4">
+        <f>$E4*I1/$E1</f>
+        <v>101.14285714285714</v>
+      </c>
+      <c r="J4">
+        <f>$E4*J1/$E1</f>
+        <v>161.82857142857145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <f>C4/C3</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="4">
+        <f>D4/D3</f>
+        <v>5.0400000000000002E-3</v>
+      </c>
+      <c r="E6" s="4">
+        <f>E4/E3</f>
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="F6" s="4">
+        <f>F4/F3</f>
+        <v>4.3828571428571432E-3</v>
+      </c>
+      <c r="G6" s="4">
+        <f>G4/G3</f>
+        <v>6.0685714285714292E-3</v>
+      </c>
+      <c r="H6" s="4">
+        <f>H4/H3</f>
+        <v>8.0914285714285723E-3</v>
+      </c>
+      <c r="I6" s="4">
+        <f>I4/I3</f>
+        <v>1.0114285714285715E-2</v>
+      </c>
+      <c r="J6" s="4">
+        <f>J4/J3</f>
+        <v>1.6182857142857145E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4">
+        <v>100</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
+      <c r="E8" s="4">
+        <v>100</v>
+      </c>
+      <c r="F8" s="4">
+        <v>100</v>
+      </c>
+      <c r="G8" s="4">
+        <v>100</v>
+      </c>
+      <c r="H8" s="4">
+        <v>100</v>
+      </c>
+      <c r="I8" s="4">
+        <v>100</v>
+      </c>
+      <c r="J8" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4">
+        <f>C8*C6</f>
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="4">
+        <f>D8*D6</f>
+        <v>0.504</v>
+      </c>
+      <c r="E9" s="4">
+        <f>E8*E6</f>
+        <v>0.23600000000000002</v>
+      </c>
+      <c r="F9" s="4">
+        <f>F8*F6</f>
+        <v>0.43828571428571433</v>
+      </c>
+      <c r="G9" s="4">
+        <f>G8*G6</f>
+        <v>0.60685714285714287</v>
+      </c>
+      <c r="H9" s="4">
+        <f>H8*H6</f>
+        <v>0.80914285714285727</v>
+      </c>
+      <c r="I9" s="4">
+        <f>I8*I6</f>
+        <v>1.0114285714285716</v>
+      </c>
+      <c r="J9" s="4">
+        <f>J8*J6</f>
+        <v>1.6182857142857145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10">
+        <v>1100</v>
+      </c>
+      <c r="F10">
+        <v>1588</v>
+      </c>
+      <c r="G10">
+        <v>1935</v>
+      </c>
+      <c r="H10">
+        <v>2192</v>
+      </c>
+      <c r="I10">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11">
+        <v>1.84</v>
+      </c>
+      <c r="F11">
+        <v>2.16</v>
+      </c>
+      <c r="G11">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="H11">
+        <v>2.44</v>
+      </c>
+      <c r="I11">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12">
+        <f>EXP((E10+466.94)/837.41)</f>
+        <v>6.4959195337489239</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:I12" si="0">EXP((F10+466.94)/837.41)</f>
+        <v>11.63390182348347</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>17.606995497589001</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>23.931484768607543</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>28.084340465669452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="D14" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="E14" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F14" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="G14" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="H14" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="I14" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="J14" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <v>33</v>
+      </c>
+      <c r="F15">
+        <v>33</v>
+      </c>
+      <c r="G15">
+        <v>33</v>
+      </c>
+      <c r="H15">
+        <v>33</v>
+      </c>
+      <c r="I15">
+        <v>33</v>
+      </c>
+      <c r="J15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4">
+        <f>C14*C15</f>
+        <v>3.2999999999999997E-6</v>
+      </c>
+      <c r="D16" s="4">
+        <f>D14*D15</f>
+        <v>3.2999999999999997E-6</v>
+      </c>
+      <c r="E16" s="4">
+        <f>E14*E15</f>
+        <v>3.2999999999999997E-6</v>
+      </c>
+      <c r="F16" s="4">
+        <f>F14*F15</f>
+        <v>3.2999999999999997E-6</v>
+      </c>
+      <c r="G16" s="4">
+        <f>G14*G15</f>
+        <v>3.2999999999999997E-6</v>
+      </c>
+      <c r="H16" s="4">
+        <f>H14*H15</f>
+        <v>3.2999999999999997E-6</v>
+      </c>
+      <c r="I16" s="4">
+        <f>I14*I15</f>
+        <v>3.2999999999999997E-6</v>
+      </c>
+      <c r="J16" s="4">
+        <f>J14*J15</f>
+        <v>3.2999999999999997E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4">
+        <f>C16*1000</f>
+        <v>3.2999999999999995E-3</v>
+      </c>
+      <c r="D17" s="4">
+        <f>D16*1000</f>
+        <v>3.2999999999999995E-3</v>
+      </c>
+      <c r="E17" s="4">
+        <f>E16*1000</f>
+        <v>3.2999999999999995E-3</v>
+      </c>
+      <c r="F17" s="4">
+        <f>F16*1000</f>
+        <v>3.2999999999999995E-3</v>
+      </c>
+      <c r="G17" s="4">
+        <f>G16*1000</f>
+        <v>3.2999999999999995E-3</v>
+      </c>
+      <c r="H17" s="4">
+        <f>H16*1000</f>
+        <v>3.2999999999999995E-3</v>
+      </c>
+      <c r="I17" s="4">
+        <f>I16*1000</f>
+        <v>3.2999999999999995E-3</v>
+      </c>
+      <c r="J17" s="4">
+        <f>J16*1000</f>
+        <v>3.2999999999999995E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4">
+        <f>C17*1000</f>
+        <v>3.2999999999999994</v>
+      </c>
+      <c r="D18" s="4">
+        <f>D17*1000</f>
+        <v>3.2999999999999994</v>
+      </c>
+      <c r="E18" s="4">
+        <f>E17*1000</f>
+        <v>3.2999999999999994</v>
+      </c>
+      <c r="F18" s="4">
+        <f>F17*1000</f>
+        <v>3.2999999999999994</v>
+      </c>
+      <c r="G18" s="4">
+        <f>G17*1000</f>
+        <v>3.2999999999999994</v>
+      </c>
+      <c r="H18" s="4">
+        <f>H17*1000</f>
+        <v>3.2999999999999994</v>
+      </c>
+      <c r="I18" s="4">
+        <f>I17*1000</f>
+        <v>3.2999999999999994</v>
+      </c>
+      <c r="J18" s="4">
+        <f>J17*1000</f>
+        <v>3.2999999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA0CE89-4A59-4C8D-A0E5-65DB02CA5D3B}">
+  <dimension ref="A3:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0.01</v>
+      </c>
+      <c r="D3">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>120</v>
+      </c>
+      <c r="D4">
+        <v>120</v>
+      </c>
+      <c r="H4">
+        <f>J4*0.000002</f>
+        <v>1.9999999999999998E-5</v>
+      </c>
+      <c r="I4">
+        <f>J4*0.004</f>
+        <v>0.04</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <f>I4^2/J4</f>
+        <v>1.6000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <f>C4/C3</f>
+        <v>12000</v>
+      </c>
+      <c r="D5">
+        <f>D4/D3</f>
+        <v>3333.3333333333335</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H6" si="0">J5*0.000002</f>
+        <v>1.9999999999999998E-4</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I6" si="1">J5*0.004</f>
+        <v>0.4</v>
+      </c>
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K6" si="2">I5^2/J5</f>
+        <v>1.6000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <f>C4^2/C5</f>
+        <v>1.2</v>
+      </c>
+      <c r="D6">
+        <f>D4^2/D5</f>
+        <v>4.3199999999999994</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>2E-3</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>1000</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f>0.036/0.000002</f>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f>30/18000</f>
+        <v>1.6666666666666668E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f>0.2/100000</f>
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f>C11*1000000</f>
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17">
+        <f>F15/F16</f>
+        <v>1.8181818181818181E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f>F17*1000</f>
+        <v>18.18181818181818</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20">
+        <f>F16*F17^2</f>
+        <v>2.1818181818181817</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>